<commit_message>
modify linux device driver
</commit_message>
<xml_diff>
--- a/Linux/DeviceDrivers/Document(important)/01.procfs.xlsx
+++ b/Linux/DeviceDrivers/Document(important)/01.procfs.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{1213F2AE-FD97-44C2-85A1-7CE21930DFAE}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD30E6DE-8DDA-403E-BCA2-816C4D5AAAAE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="procfs" sheetId="2" r:id="rId1"/>
-    <sheet name="procfs的套路" sheetId="3" r:id="rId2"/>
+    <sheet name="procfs_sam" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>fs/proc/generic.c
 EXPORT_SYMBOL:
@@ -212,22 +212,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>struct proc_dir_entry *ylmtest_dir = proc_mkdir("ylmtestdir", NULL);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>static int ylmtest_proc_read(struct seq_file * m, void* vp);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>static ssize_t ylmtest_proc_write(struct file *file, const char *buffer, size_t count, loff_t *loff);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>static int ylmtest_proc_open(struct inode *inode, struct file *file);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>seq_printf()</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -240,30 +224,12 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>return single_open(file, &amp;ylmtest_proc_read, NULL);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">    .open = ylmtest_proc_open,</t>
-  </si>
-  <si>
     <t xml:space="preserve">    .read = seq_read,</t>
   </si>
   <si>
-    <t xml:space="preserve">    .write = ylmtest_proc_write,</t>
-  </si>
-  <si>
     <t>};</t>
   </si>
   <si>
-    <t>static struct file_operations ylmtest_proc_file_operations = {</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>struct proc_dir_entry *ylmtest_entry = proc_create_data("ylmtest", 0666, ylmtest_dir, &amp;ylmtest_proc_file_operations, NULL);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">3. </t>
     </r>
@@ -299,11 +265,55 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>remove_proc_entry("ylmtest", "ylmtest_dir");</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>remove_proc_entry("ylmtest_dir", NULL);</t>
+    <t>################################ procfs ################################</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>struct proc_dir_entry *test_proc_dir = proc_mkdir("test_proc_dir", NULL);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>static int test_proc_read(struct seq_file * m, void* vp);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>static ssize_t test_proc_write(struct file *file, const char *buffer, size_t count, loff_t *loff);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>static int test_proc_open(struct inode *inode, struct file *file);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">    .open = test_proc_open,</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">    .write = test_proc_write,</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>struct proc_dir_entry *test_proc_entry;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>test_proc_entry = proc_create_data("test_proc", 0666, test_proc_dir, &amp;test_proc_fops, NULL);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>static struct file_operations test_proc_fops = {</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>remove_proc_entry("test_proc", "test_proc_dir");</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>remove_proc_entry("test_proc_dir", NULL);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>return single_open(file, &amp;test_proc_read, NULL);</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -676,25 +686,25 @@
   <dimension ref="B1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="100.625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="100.6640625" style="1" customWidth="1"/>
     <col min="5" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B1" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
     </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
@@ -705,7 +715,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:4" ht="276" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:4" ht="276" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
@@ -714,7 +724,7 @@
       </c>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="2:4" ht="192" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:4" ht="240" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
@@ -731,110 +741,120 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00ACB836-2E73-4677-B951-324A246E1F0A}">
-  <dimension ref="B2:C26"/>
+  <dimension ref="B2:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AO26" sqref="AO26"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="AB23" sqref="AB23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="2.6640625" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="2.625" style="1"/>
+    <col min="1" max="16384" width="2.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B3" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C4" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B7" s="1" t="s">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C7" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D8" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C8" s="1" t="s">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D9" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C11" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D12" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C14" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D15" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C17" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C18" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C19" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C20" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C21" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C23" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C24" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C9" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C11" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B12" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C13" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B15" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B17" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B18" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B19" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B21" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B24" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B25" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B26" s="1" t="s">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C27" s="1" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C28" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>